<commit_message>
updated the PCB to have two functioning channels, V1.7
</commit_message>
<xml_diff>
--- a/BOM/Bittele/71407A1_BOM_SL_2022-01-21.xlsx
+++ b/BOM/Bittele/71407A1_BOM_SL_2022-01-21.xlsx
@@ -1515,7 +1515,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1573,6 +1573,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1664,10 +1672,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1700,6 +1709,10 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1709,7 +1722,8 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="42">
@@ -5663,8 +5677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6076,7 +6090,7 @@
       <c r="E3" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="26" t="s">
         <v>53</v>
       </c>
       <c r="G3" s="11" t="s">
@@ -6256,7 +6270,7 @@
       <c r="E4" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="29" t="s">
         <v>69</v>
       </c>
       <c r="G4" s="13" t="s">
@@ -6436,7 +6450,7 @@
       <c r="E5" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="26" t="s">
         <v>84</v>
       </c>
       <c r="G5" s="11" t="s">
@@ -6616,7 +6630,7 @@
       <c r="E6" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="29" t="s">
         <v>105</v>
       </c>
       <c r="G6" s="13" t="s">
@@ -6796,7 +6810,7 @@
       <c r="E7" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="26" t="s">
         <v>121</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -6974,7 +6988,7 @@
       <c r="E8" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="29" t="s">
         <v>132</v>
       </c>
       <c r="G8" s="13" t="s">
@@ -7154,7 +7168,7 @@
       <c r="E9" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="26" t="s">
         <v>149</v>
       </c>
       <c r="G9" s="11" t="s">
@@ -7334,7 +7348,7 @@
       <c r="E10" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="29" t="s">
         <v>165</v>
       </c>
       <c r="G10" s="13" t="s">
@@ -7514,7 +7528,7 @@
       <c r="E11" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="26" t="s">
         <v>179</v>
       </c>
       <c r="G11" s="11" t="s">
@@ -7694,7 +7708,7 @@
       <c r="E12" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="29" t="s">
         <v>198</v>
       </c>
       <c r="G12" s="13" t="s">
@@ -7874,7 +7888,7 @@
       <c r="E13" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="26" t="s">
         <v>219</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -8054,7 +8068,7 @@
       <c r="E14" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G14" s="13" t="s">
@@ -8234,7 +8248,7 @@
       <c r="E15" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="29" t="s">
         <v>275</v>
       </c>
       <c r="G15" s="13" t="s">
@@ -8414,7 +8428,7 @@
       <c r="E16" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="26" t="s">
         <v>296</v>
       </c>
       <c r="G16" s="11" t="s">
@@ -8594,7 +8608,7 @@
       <c r="E17" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="29" t="s">
         <v>313</v>
       </c>
       <c r="G17" s="13" t="s">
@@ -8774,7 +8788,7 @@
       <c r="E18" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="29" t="s">
         <v>328</v>
       </c>
       <c r="G18" s="13" t="s">
@@ -8954,7 +8968,7 @@
       <c r="E19" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="26" t="s">
         <v>349</v>
       </c>
       <c r="G19" s="11" t="s">
@@ -9134,7 +9148,7 @@
       <c r="E20" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="29" t="s">
         <v>368</v>
       </c>
       <c r="G20" s="13" t="s">
@@ -9314,7 +9328,7 @@
       <c r="E21" s="17" t="s">
         <v>377</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="28" t="s">
         <v>379</v>
       </c>
       <c r="G21" s="17" t="s">
@@ -9498,7 +9512,7 @@
       <c r="E22" s="21" t="s">
         <v>390</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="27" t="s">
         <v>392</v>
       </c>
       <c r="G22" s="21" t="s">
@@ -9682,7 +9696,7 @@
       <c r="E23" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="26" t="s">
         <v>402</v>
       </c>
       <c r="G23" s="11" t="s">
@@ -9847,10 +9861,10 @@
       <c r="BJ23" s="9"/>
     </row>
     <row r="24" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AV24" s="26" t="s">
+      <c r="AV24" s="30" t="s">
         <v>473</v>
       </c>
-      <c r="AW24" s="26"/>
+      <c r="AW24" s="30"/>
       <c r="AX24" s="24">
         <f>SUM(AX2:AX23)</f>
         <v>299.57199999999995</v>
@@ -9880,29 +9894,29 @@
       </c>
     </row>
     <row r="26" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AV26" s="27" t="s">
+      <c r="AV26" s="31" t="s">
         <v>474</v>
       </c>
-      <c r="AW26" s="27"/>
+      <c r="AW26" s="31"/>
       <c r="AX26" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AV27" s="28" t="s">
+      <c r="AV27" s="32" t="s">
         <v>475</v>
       </c>
-      <c r="AW27" s="28"/>
+      <c r="AW27" s="32"/>
       <c r="AX27" s="24">
         <f>SUM(AX24:AX26)</f>
         <v>299.57199999999995</v>
       </c>
     </row>
     <row r="28" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AV28" s="29" t="s">
+      <c r="AV28" s="33" t="s">
         <v>476</v>
       </c>
-      <c r="AW28" s="29"/>
+      <c r="AW28" s="33"/>
       <c r="AX28" s="25">
         <f>(AX27/10)</f>
         <v>29.957199999999993</v>
@@ -9922,8 +9936,31 @@
   <conditionalFormatting sqref="BB1:BC1">
     <cfRule type="duplicateValues" dxfId="0" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="F23" r:id="rId1"/>
+    <hyperlink ref="F22" r:id="rId2"/>
+    <hyperlink ref="F21" r:id="rId3"/>
+    <hyperlink ref="F20" r:id="rId4"/>
+    <hyperlink ref="F19" r:id="rId5"/>
+    <hyperlink ref="F18" r:id="rId6"/>
+    <hyperlink ref="F17" r:id="rId7"/>
+    <hyperlink ref="F16" r:id="rId8"/>
+    <hyperlink ref="F15" r:id="rId9"/>
+    <hyperlink ref="F14" r:id="rId10"/>
+    <hyperlink ref="F13" r:id="rId11"/>
+    <hyperlink ref="F12" r:id="rId12"/>
+    <hyperlink ref="F11" r:id="rId13"/>
+    <hyperlink ref="F10" r:id="rId14"/>
+    <hyperlink ref="F9" r:id="rId15"/>
+    <hyperlink ref="F8" r:id="rId16"/>
+    <hyperlink ref="F7" r:id="rId17"/>
+    <hyperlink ref="F6" r:id="rId18"/>
+    <hyperlink ref="F5" r:id="rId19"/>
+    <hyperlink ref="F4" r:id="rId20"/>
+    <hyperlink ref="F3" r:id="rId21"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>